<commit_message>
mejoras en errores, creo que me queda sinc_todo
</commit_message>
<xml_diff>
--- a/app/datos/cierre_caja/resultado_panda.xlsx
+++ b/app/datos/cierre_caja/resultado_panda.xlsx
@@ -7,16 +7,323 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Velázquez" sheetId="1" r:id="rId1"/>
+    <sheet name="MG Norte" sheetId="2" r:id="rId2"/>
+    <sheet name="MG" sheetId="3" r:id="rId3"/>
+    <sheet name="SOL-Bombonería" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="97">
+  <si>
+    <t>Tienda</t>
+  </si>
+  <si>
+    <t>Nombre_TPV</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>cierre_tpv_desc</t>
+  </si>
+  <si>
+    <t>Nombre_MdP</t>
+  </si>
+  <si>
+    <t>total_ventas</t>
+  </si>
+  <si>
+    <t>total_operaciones</t>
+  </si>
+  <si>
+    <t>Velázquez</t>
+  </si>
+  <si>
+    <t>BAR</t>
+  </si>
+  <si>
+    <t>SERVIDOR TIENDA</t>
+  </si>
+  <si>
+    <t>05/10/2024</t>
+  </si>
+  <si>
+    <t>Mañana</t>
+  </si>
+  <si>
+    <t>Tarde</t>
+  </si>
+  <si>
+    <t>EUROS</t>
+  </si>
+  <si>
+    <t>TARJETA VISA</t>
+  </si>
+  <si>
+    <t>GLOVO</t>
+  </si>
+  <si>
+    <t>SMS</t>
+  </si>
+  <si>
+    <t>295,50</t>
+  </si>
+  <si>
+    <t>857,99</t>
+  </si>
+  <si>
+    <t>563,28</t>
+  </si>
+  <si>
+    <t>73,80</t>
+  </si>
+  <si>
+    <t>1351,34</t>
+  </si>
+  <si>
+    <t>957,52</t>
+  </si>
+  <si>
+    <t>95,30</t>
+  </si>
+  <si>
+    <t>3,60</t>
+  </si>
+  <si>
+    <t>2331,75</t>
+  </si>
+  <si>
+    <t>553,54</t>
+  </si>
+  <si>
+    <t>1098,34</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>207</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>MG Norte</t>
+  </si>
+  <si>
+    <t>SERVIDOR NORTE</t>
+  </si>
+  <si>
+    <t>TPV III (Barra)</t>
+  </si>
+  <si>
+    <t>REMOTO TIENDA</t>
+  </si>
+  <si>
+    <t>RAPID EXPRESS</t>
+  </si>
+  <si>
+    <t>TRANSFERENCIA</t>
+  </si>
+  <si>
+    <t>136,70</t>
+  </si>
+  <si>
+    <t>114,70</t>
+  </si>
+  <si>
+    <t>740,89</t>
+  </si>
+  <si>
+    <t>131,72</t>
+  </si>
+  <si>
+    <t>387,60</t>
+  </si>
+  <si>
+    <t>798,75</t>
+  </si>
+  <si>
+    <t>35,20</t>
+  </si>
+  <si>
+    <t>769,16</t>
+  </si>
+  <si>
+    <t>375,50</t>
+  </si>
+  <si>
+    <t>4,90</t>
+  </si>
+  <si>
+    <t>925,66</t>
+  </si>
+  <si>
+    <t>1057,10</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>MORALEJA</t>
+  </si>
+  <si>
+    <t>50,70</t>
+  </si>
+  <si>
+    <t>241,60</t>
+  </si>
+  <si>
+    <t>151,71</t>
+  </si>
+  <si>
+    <t>576,52</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>SOL-Bombonería</t>
+  </si>
+  <si>
+    <t>BOMBONERIA</t>
+  </si>
+  <si>
+    <t>TIENDA</t>
+  </si>
+  <si>
+    <t>TICKET RESTAURANT</t>
+  </si>
+  <si>
+    <t>619,86</t>
+  </si>
+  <si>
+    <t>1344,46</t>
+  </si>
+  <si>
+    <t>1676,10</t>
+  </si>
+  <si>
+    <t>2673,20</t>
+  </si>
+  <si>
+    <t>994,50</t>
+  </si>
+  <si>
+    <t>2654,40</t>
+  </si>
+  <si>
+    <t>2039,50</t>
+  </si>
+  <si>
+    <t>28,00</t>
+  </si>
+  <si>
+    <t>4214,61</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>164</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>329</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -32,7 +339,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,12 +347,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,12 +665,972 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>